<commit_message>
added Logo in ProjectDocumentation/HomeAutomation_1_Logo.PNG
</commit_message>
<xml_diff>
--- a/Documentation/ProjectDocumentation/Website_template.xlsx
+++ b/Documentation/ProjectDocumentation/Website_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Documents\Schule\3_Semester\PRO2\SemProjekt\Projekt_HomeAutomation\p11\Documentation\ProjectDocumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hagenberg_FH\3. Semester\Semester Projekt\Home Automation\p11\Documentation\ProjectDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66553A2C-B52A-4FE1-8BF7-0AAD71DBE622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB55B6-1F5D-4C9B-9886-A98CE8714166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="330" windowWidth="27240" windowHeight="13150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Liste der Namen der Studierenden, die an diesem Projekt mitarbeiten, mit Komma getrennt.</t>
   </si>
   <si>
-    <t>Bild1.jpg,Bild2.png,Bild3.gif</t>
-  </si>
-  <si>
     <t>Ausfüllhinweise: Für 1 Projekt muss jeweils 1 Zeile ausgefüllt werden. Zu verwenden ist die obige Zeile mit den Musterdaten. Die ausgeblendeten Spalten sollen nicht eingeblendet werden.</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   <si>
     <t>Mit Hilfe unserer Home Automation Applikation soll auf ein auf dem Benutzer abgestimmte Aktion ausgeführt werden. In unserem Fall, sobald der Benutzer seinen Raum betritt, wird er von seiner Webcam, die auf einem eigenen Raspberry Pi angehängt ist, erfasst und mit der OpenCV Bibliothek und unserem Skript erkannt. Daraufhin schickt unsere Applikation eine Anfrage an unseren Raspberry Pi Server mithilfe von Webhooks. Auf unserem Server läuft das Home Assistant Betriebssystem, das diese Anfrage erhält. Unser Server bearbeitet diese Anfrage und führt die darauffolgende Aktion durch. Der Server schickt anschließend den auszuführenden Befehl (z.B. Fernseher einschalten) weiter an seinen Logitech Harmony Hub. Dieser fungiert als Ersatz für die Fernbedienung und steuert den Fernseher mit Infrarot.
 Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext.</t>
+  </si>
+  <si>
+    <t>HomeAutomation_1_Logo.png</t>
   </si>
 </sst>
 </file>
@@ -272,33 +272,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,34 +641,34 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="39.33203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="3.5546875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="39.6640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="30.5546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.453125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="39.36328125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="3.54296875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.36328125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="39.6328125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="30.54296875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14.36328125" customWidth="1"/>
+    <col min="20" max="20" width="9.08984375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -732,34 +732,34 @@
     </row>
     <row r="2" spans="1:20" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>40</v>
+      <c r="O2" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="T2" s="6">
         <v>1</v>
@@ -769,189 +769,189 @@
     <row r="4" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="A6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="B7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="B8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="B12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="B13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="9"/>
+      <c r="A14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="10"/>
     </row>
   </sheetData>
   <sheetProtection password="E579" sheet="1" selectLockedCells="1"/>
@@ -979,7 +979,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -993,7 +993,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>